<commit_message>
test update output column
</commit_message>
<xml_diff>
--- a/templates/dataplant/3ASY01_RNASeq.xlsx
+++ b/templates/dataplant/3ASY01_RNASeq.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\SWATE_templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\Swate-templates_FORK\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5B9723-FC1D-4BAE-8066-AB3DB41DE93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE62BD52-C841-48DE-B7B4-74D2AD7ECEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="19110" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6165" yWindow="2340" windowWidth="22785" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3ASY01_RNASeq" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="176">
   <si>
     <t>Source Name</t>
   </si>
@@ -748,6 +748,9 @@
   <si>
     <t>Authors Role Term Source REF</t>
   </si>
+  <si>
+    <t>Raw Data File</t>
+  </si>
 </sst>
 </file>
 
@@ -756,7 +759,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;microgram&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -784,12 +787,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1114,7 +1111,7 @@
     <tableColumn id="40" xr3:uid="{2AFADBEA-D2CA-4459-8C9D-3DC3FA4E226B}" name="Parameter [Raw data file format]" dataDxfId="3"/>
     <tableColumn id="41" xr3:uid="{CC4AA291-442E-477D-A16A-36D7D1CB0B50}" name="Term Source REF (NFDI4PSO:0000021)" dataDxfId="2"/>
     <tableColumn id="42" xr3:uid="{E3E37F73-63D0-4BEE-A350-CE87A85AB65F}" name="Term Accession Number (NFDI4PSO:0000021)" dataDxfId="1"/>
-    <tableColumn id="43" xr3:uid="{2365BEFE-DF52-4424-991C-DFFA0DF1C8E9}" name="Data File Name" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{47A34C5D-CBA3-4D67-95F8-EF106ACCAA38}" name="Raw Data File" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1418,7 +1415,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="631" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="512" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="643" row="3">
@@ -1451,55 +1448,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AP2" sqref="AP2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="42" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="31" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7.140625" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="57" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="57.42578125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="34" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="32" max="32" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="41.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="41.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="35" max="35" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="44.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="45.140625" style="14" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="41" max="41" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="33" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="44" max="44" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
@@ -1636,7 +1635,7 @@
         <v>40</v>
       </c>
       <c r="AS1" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.25">
@@ -1745,7 +1744,7 @@
       <c r="AR2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AS2" s="1"/>
+      <c r="AS2" s="14"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1825,7 +1824,7 @@
       <c r="AR3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AS3" s="1"/>
+      <c r="AS3" s="14"/>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1890,7 +1889,7 @@
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
-      <c r="AS4" s="1"/>
+      <c r="AS4" s="14"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
@@ -1931,7 +1930,7 @@
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
-      <c r="AS5" s="1"/>
+      <c r="AS5" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1946,7 +1945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCFAEC7-2CE0-4201-B33B-152C0680AE1F}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>